<commit_message>
Search customer by Email test case
</commit_message>
<xml_diff>
--- a/testData/LoginData_nopCommerceApp.xlsx
+++ b/testData/LoginData_nopCommerceApp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quicket-Solutions\PycharmProjects\nopcommerceApp\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Automation_Practice\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437F7207-9FEC-4C4E-84CC-D74846ED8B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA966155-6111-4BEE-9999-61D37F4C46FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E986745A-E480-4B8F-A2D0-E89D2654A24D}"/>
   </bookViews>
@@ -16,28 +16,17 @@
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Customer_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>username</t>
   </si>
@@ -96,12 +85,6 @@
     <t>test123</t>
   </si>
   <si>
-    <t>Nishchay</t>
-  </si>
-  <si>
-    <t>Angra</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -114,9 +97,6 @@
     <t>Test_123</t>
   </si>
   <si>
-    <t>Rajat</t>
-  </si>
-  <si>
     <t>Kapoor</t>
   </si>
   <si>
@@ -138,9 +118,6 @@
     <t>test@123</t>
   </si>
   <si>
-    <t>Seema</t>
-  </si>
-  <si>
     <t>Sharma</t>
   </si>
   <si>
@@ -159,18 +136,12 @@
     <t>test#123</t>
   </si>
   <si>
-    <t>Manu</t>
-  </si>
-  <si>
     <t>Chopra</t>
   </si>
   <si>
     <t>Test_12345</t>
   </si>
   <si>
-    <t>Raman</t>
-  </si>
-  <si>
     <t>Gupta</t>
   </si>
   <si>
@@ -190,6 +161,42 @@
   </si>
   <si>
     <t>Test store 2</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Darren</t>
+  </si>
+  <si>
+    <t>Bravo</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Meena</t>
+  </si>
+  <si>
+    <t>Vihan</t>
+  </si>
+  <si>
+    <t>Saumya</t>
+  </si>
+  <si>
+    <t>darrbravo@gmail.com</t>
+  </si>
+  <si>
+    <t>rohkapoor@gmail.com</t>
+  </si>
+  <si>
+    <t>meesharma@gmail.com</t>
+  </si>
+  <si>
+    <t>sauchopra@gmail.com</t>
+  </si>
+  <si>
+    <t>vihgupta@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -265,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -288,12 +295,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -310,6 +328,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -702,10 +724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17BE99B-FA81-45DA-92E4-EAB00F4969BF}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,9 +739,10 @@
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -750,169 +773,193 @@
       <c r="J1" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="6">
         <v>36086</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="6">
         <v>36697</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E4" s="6">
         <v>35536</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6">
         <v>37572</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6">
         <v>34588</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{42488299-979F-4430-82AB-8453758A2540}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{B949D7B3-BB06-49B9-8889-453C3D284AD4}"/>
+    <hyperlink ref="K3:K6" r:id="rId3" display="dbravo@gmail.com" xr:uid="{5FA63606-F4CB-4549-A182-ACDA33B68C56}"/>
+    <hyperlink ref="K3" r:id="rId4" xr:uid="{BDDBC0F2-D6F5-437D-845D-877458E6075C}"/>
+    <hyperlink ref="K4" r:id="rId5" xr:uid="{DC2AEC24-4CB0-4F72-877E-1DEB4B8B1401}"/>
+    <hyperlink ref="K5" r:id="rId6" xr:uid="{43C0AC17-4EFC-4D6B-9DCB-C778A2C97963}"/>
+    <hyperlink ref="K6" r:id="rId7" xr:uid="{4532DF18-B229-4983-8BAA-85C7914E175C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification in Search customer by Email test case
</commit_message>
<xml_diff>
--- a/testData/LoginData_nopCommerceApp.xlsx
+++ b/testData/LoginData_nopCommerceApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Automation_Practice\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA966155-6111-4BEE-9999-61D37F4C46FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BABF64-EC9D-4045-93A2-B1942D99C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E986745A-E480-4B8F-A2D0-E89D2654A24D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -103,9 +103,6 @@
     <t>company1</t>
   </si>
   <si>
-    <t>Guests</t>
-  </si>
-  <si>
     <t>Vendors</t>
   </si>
   <si>
@@ -166,15 +163,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>Darren</t>
-  </si>
-  <si>
-    <t>Bravo</t>
-  </si>
-  <si>
-    <t>Rohan</t>
-  </si>
-  <si>
     <t>Meena</t>
   </si>
   <si>
@@ -184,19 +172,28 @@
     <t>Saumya</t>
   </si>
   <si>
-    <t>darrbravo@gmail.com</t>
-  </si>
-  <si>
-    <t>rohkapoor@gmail.com</t>
-  </si>
-  <si>
-    <t>meesharma@gmail.com</t>
-  </si>
-  <si>
-    <t>sauchopra@gmail.com</t>
-  </si>
-  <si>
-    <t>vihgupta@gmail.com</t>
+    <t>meensharma@gmail.com</t>
+  </si>
+  <si>
+    <t>saumchopra@gmail.com</t>
+  </si>
+  <si>
+    <t>vihagupta@gmail.com</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Goyal</t>
+  </si>
+  <si>
+    <t>Manish</t>
+  </si>
+  <si>
+    <t>ramgoyal@gmail.com</t>
+  </si>
+  <si>
+    <t>makapoor@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -727,7 +724,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +736,7 @@
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -774,7 +771,7 @@
         <v>17</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -782,10 +779,10 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -797,19 +794,19 @@
         <v>21</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -817,7 +814,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>23</v>
@@ -832,100 +829,100 @@
         <v>24</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E4" s="6">
         <v>35536</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="6">
         <v>37572</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -934,20 +931,20 @@
         <v>34588</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Search customer by Name test case
</commit_message>
<xml_diff>
--- a/testData/LoginData_nopCommerceApp.xlsx
+++ b/testData/LoginData_nopCommerceApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Automation_Practice\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BABF64-EC9D-4045-93A2-B1942D99C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DF1F6D-AE36-4006-B94E-685AE807EBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E986745A-E480-4B8F-A2D0-E89D2654A24D}"/>
   </bookViews>
@@ -172,15 +172,6 @@
     <t>Saumya</t>
   </si>
   <si>
-    <t>meensharma@gmail.com</t>
-  </si>
-  <si>
-    <t>saumchopra@gmail.com</t>
-  </si>
-  <si>
-    <t>vihagupta@gmail.com</t>
-  </si>
-  <si>
     <t>Ramesh</t>
   </si>
   <si>
@@ -190,10 +181,19 @@
     <t>Manish</t>
   </si>
   <si>
-    <t>ramgoyal@gmail.com</t>
-  </si>
-  <si>
-    <t>makapoor@gmail.com</t>
+    <t>manikapoor@gmail.com</t>
+  </si>
+  <si>
+    <t>meenasharma1@gmail.com</t>
+  </si>
+  <si>
+    <t>saumyachopra@gmail.com</t>
+  </si>
+  <si>
+    <t>vihangupta1@gmail.com</t>
+  </si>
+  <si>
+    <t>rameshgoyal@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -724,7 +724,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,10 +779,10 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -806,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -814,7 +814,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>23</v>
@@ -841,7 +841,7 @@
         <v>20</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -876,7 +876,7 @@
         <v>20</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
         <v>20</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -944,7 +944,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>